<commit_message>
Plan de Trabajo en Excel
</commit_message>
<xml_diff>
--- a/plan_de_trabajo.xlsx
+++ b/plan_de_trabajo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FEDESOFT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo.FonsecaC\Desktop\grupo6\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
   <si>
     <t>APP MEDIO AMBIENTE ENFOCADO A ZONAS PROTEGIDAS</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Directorio de sitios de reciclaje</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Empresas</t>
   </si>
   <si>
@@ -56,18 +53,6 @@
     <t>Foro-envio de datos on line</t>
   </si>
   <si>
-    <t>El administrador ingresa actividades y son enviadas por correo a los usuarios registrados</t>
-  </si>
-  <si>
-    <t>Actividad a la comunidad envío de correo a los registrados</t>
-  </si>
-  <si>
-    <t>Solicitudes de actividad de empresa</t>
-  </si>
-  <si>
-    <t>Formulario de actividad y link para inscrpcion</t>
-  </si>
-  <si>
     <t>Envío de imagen</t>
   </si>
   <si>
@@ -89,9 +74,6 @@
     <t>Visitantes -Registrados</t>
   </si>
   <si>
-    <t>Videos y tutoriales de temas relacionados con el reciclaje</t>
-  </si>
-  <si>
     <t>Todos</t>
   </si>
   <si>
@@ -104,10 +86,133 @@
     <t>Realizar denuncias en tiempo real</t>
   </si>
   <si>
-    <t xml:space="preserve">Usar apis o menejo de maps para indicar los puntos donde se  pueden lelvar los elemetos  a Reciclar </t>
-  </si>
-  <si>
-    <t>Se toman imágenes y se suben a la aplicación van ganando puntos a medida que suban nuevas especies, Denuncias basuras o daños en ecosistema, elusuario con más datos recolectados va sumando puntos y  gana premio, entregado al final de la visitas diarias. Pude ser individual o por  grupos seggún defina el administrador</t>
+    <t>TABLA</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>TABLA (1)</t>
+  </si>
+  <si>
+    <t>USUARIOS</t>
+  </si>
+  <si>
+    <t>DESCRIPCION</t>
+  </si>
+  <si>
+    <t>FECHA_ACTIVIDAD</t>
+  </si>
+  <si>
+    <t>ENVIAR A:</t>
+  </si>
+  <si>
+    <t>CAMPOS</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>CORREO_USUARIO</t>
+  </si>
+  <si>
+    <t>NOMBRES APELLIDOS</t>
+  </si>
+  <si>
+    <t>TIPO_USUARIO</t>
+  </si>
+  <si>
+    <t>ID_USUARIO</t>
+  </si>
+  <si>
+    <t>NUMBER</t>
+  </si>
+  <si>
+    <t>MAIL</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+  </si>
+  <si>
+    <t>TABLA (2)</t>
+  </si>
+  <si>
+    <t>REGISTRO</t>
+  </si>
+  <si>
+    <t>ACTIVIDADES</t>
+  </si>
+  <si>
+    <t>NOMBRE_ACTIVIDAD</t>
+  </si>
+  <si>
+    <t>ENVIAR :</t>
+  </si>
+  <si>
+    <t>URL DE VIDEO</t>
+  </si>
+  <si>
+    <t>Enviar por tipo de usuario</t>
+  </si>
+  <si>
+    <t>Envío individual</t>
+  </si>
+  <si>
+    <t>Ingresar actividad</t>
+  </si>
+  <si>
+    <t>link para inscribir el grupo- esta limitado</t>
+  </si>
+  <si>
+    <t>seleccionar correo quien se envía - en lista los 3 principales u opcion de digitar un correo nuevo</t>
+  </si>
+  <si>
+    <t>fecha_inscripcion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usar apis o manejo de maps para indicar los puntos donde se  pueden llevar los elemetos  a Reciclar </t>
+  </si>
+  <si>
+    <t>Se toman imágenes y se suben a la aplicación van ganando puntos a medida que suban nuevas especies, Denuncias basuras o daños en ecosistema, el usuario con más datos recolectados va sumando puntos y  gana premio, entregado al final de la visitas diarias. Pude ser individual o por  grupos según se defina el administrador</t>
+  </si>
+  <si>
+    <t>Ingresa: correo ,nombr, apellidos y tipo de usuario</t>
+  </si>
+  <si>
+    <t>Denuncias</t>
+  </si>
+  <si>
+    <t>DENUNCIAS</t>
+  </si>
+  <si>
+    <t>DENUNCIA</t>
+  </si>
+  <si>
+    <t>FOTOGRAFIA</t>
+  </si>
+  <si>
+    <t>TABLA (3)</t>
+  </si>
+  <si>
+    <t>GANAPUNTOS</t>
+  </si>
+  <si>
+    <t>Usuario (1)</t>
+  </si>
+  <si>
+    <t>Tipo_Usuario(2)</t>
+  </si>
+  <si>
+    <t>TABLA (4)</t>
+  </si>
+  <si>
+    <t>Actividades(3)</t>
+  </si>
+  <si>
+    <t>Aprende(4)</t>
+  </si>
+  <si>
+    <t>APRENDE</t>
   </si>
 </sst>
 </file>
@@ -156,48 +261,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -205,26 +273,17 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -234,7 +293,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -242,12 +301,23 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -255,19 +325,54 @@
     <border>
       <left/>
       <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -276,35 +381,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,178 +709,461 @@
     <col min="1" max="1" width="53.33203125" customWidth="1"/>
     <col min="2" max="2" width="150.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="22"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="21"/>
+      <c r="B6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="22"/>
+      <c r="B7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="21"/>
+      <c r="B9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="21"/>
+      <c r="B10" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="22"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="19" t="s">
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="21"/>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="22"/>
+      <c r="B14" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="15"/>
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="15"/>
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="5"/>
+      <c r="B22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="5"/>
+      <c r="B26" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="C26" s="6"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+      <c r="B30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="5"/>
+      <c r="B31" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="3"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="11" t="s">
+      <c r="C34" s="4"/>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="5"/>
+      <c r="B36" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="3"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="5"/>
+      <c r="B39" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="13" t="s">
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="4"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="3"/>
+      <c r="B42" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="3"/>
+      <c r="B43" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="5"/>
+      <c r="B44" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="3"/>
+      <c r="B47" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="3"/>
+      <c r="B48" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" s="4"/>
+    </row>
+    <row r="49" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="5"/>
+      <c r="B49" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A3:A4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>